<commit_message>
update new query in SSMS
</commit_message>
<xml_diff>
--- a/StudentList.xlsx
+++ b/StudentList.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27413"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT University\DPI202\github\StudentManagementDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7076F42A-1260-4E82-ADEA-54BA819E25A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{7076F42A-1260-4E82-ADEA-54BA819E25A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6289FA8C-0C0E-4E90-89C0-0612DEA37F9D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C5753F7D-290E-43CF-B893-8C0D3F93B633}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="150">
+  <si>
+    <t>họ và tên</t>
+  </si>
+  <si>
+    <t>mã số sinh viên</t>
+  </si>
+  <si>
+    <t>giới tính</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>cơ sở đào tạo</t>
+  </si>
+  <si>
+    <t>chuyên ngành</t>
+  </si>
   <si>
     <t xml:space="preserve">Bach Bao Yen </t>
   </si>
@@ -44,81 +63,63 @@
     <t>CS182215</t>
   </si>
   <si>
+    <t>Female</t>
+  </si>
+  <si>
     <t>yenbbcs182215@fpt.edu.vn</t>
   </si>
   <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Kỳ Anh Minh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">se180117 </t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>minhnkase173338@fpt.edu.vn</t>
+  </si>
+  <si>
     <t>HCM</t>
   </si>
   <si>
-    <t>cơ sở đào tạo</t>
-  </si>
-  <si>
-    <t>chuyên ngành</t>
-  </si>
-  <si>
-    <t>CT</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
     <t>SE</t>
   </si>
   <si>
+    <t xml:space="preserve">Vo Lam Son </t>
+  </si>
+  <si>
+    <t xml:space="preserve">se170119 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sonvlse170119@fpt.edu.vn </t>
+  </si>
+  <si>
     <t xml:space="preserve">HCM </t>
   </si>
   <si>
+    <t xml:space="preserve">Chauvreau Phuong  </t>
+  </si>
+  <si>
+    <t>ca181277</t>
+  </si>
+  <si>
+    <t>phuongcca181277@fpt.edu.vn</t>
+  </si>
+  <si>
     <t>CA</t>
   </si>
   <si>
     <t>Bui Truong Thinh</t>
   </si>
   <si>
-    <t>mã số sinh viên</t>
-  </si>
-  <si>
-    <t>giới tính</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>họ và tên</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>minhnkase173338@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>phuongcca181277@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">se180117 </t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">se170119 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sonvlse170119@fpt.edu.vn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vo Lam Son </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Kỳ Anh Minh </t>
-  </si>
-  <si>
-    <t>ca181277</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chauvreau Phuong  </t>
-  </si>
-  <si>
     <t>ca180528</t>
   </si>
   <si>
@@ -128,6 +129,9 @@
     <t>Bui Xuan My</t>
   </si>
   <si>
+    <t>ce180953</t>
+  </si>
+  <si>
     <t>mybxce180953@fpt.edu.vn</t>
   </si>
   <si>
@@ -137,69 +141,66 @@
     <t>Cao Hoang Quy</t>
   </si>
   <si>
-    <t>ce180953</t>
+    <t>cs180845</t>
   </si>
   <si>
     <t>quychcs180845@fpt.edu.vn</t>
   </si>
   <si>
-    <t>cs180845</t>
-  </si>
-  <si>
     <t>Chung Ngoc Quynh</t>
   </si>
   <si>
+    <t>ce180591</t>
+  </si>
+  <si>
     <t>quynhcnce180591@fpt.edu.vn</t>
   </si>
   <si>
-    <t>ce180591</t>
-  </si>
-  <si>
     <t>Dam Khanh Linh</t>
   </si>
   <si>
+    <t>ca181738</t>
+  </si>
+  <si>
     <t>linhdkca181738@fpt.edu.vn</t>
   </si>
   <si>
-    <t>ca181738</t>
-  </si>
-  <si>
     <t>Dang Hao</t>
   </si>
   <si>
+    <t>cs181917</t>
+  </si>
+  <si>
     <t>haodcs181917@fpt.edu.vn</t>
   </si>
   <si>
-    <t>cs181917</t>
-  </si>
-  <si>
     <t>Huynh Hoang Ty</t>
   </si>
   <si>
+    <t>ce180191</t>
+  </si>
+  <si>
     <t>tyhhce180191@fpt.edu.vn</t>
   </si>
   <si>
-    <t>ce180191</t>
-  </si>
-  <si>
     <t>Ho Dao Ty</t>
   </si>
   <si>
+    <t>se183975</t>
+  </si>
+  <si>
     <t>tyhdse183975@fpt.edu.vn</t>
   </si>
   <si>
-    <t>se183975</t>
-  </si>
-  <si>
     <t>Ha Gia Manh </t>
   </si>
   <si>
+    <t>he176443</t>
+  </si>
+  <si>
     <t>manhhghe176443@fpt.edu.vn</t>
   </si>
   <si>
-    <t>he176443</t>
-  </si>
-  <si>
     <t>HL</t>
   </si>
   <si>
@@ -209,268 +210,283 @@
     <t>Dao Quang Nguyen</t>
   </si>
   <si>
+    <t>he176610</t>
+  </si>
+  <si>
     <t>nguyendqhe176610@fpt.edu.vn</t>
   </si>
   <si>
-    <t>he176610</t>
-  </si>
-  <si>
     <t>Phan Duy Anh</t>
   </si>
   <si>
+    <t>CE190127</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>AnhPD.CE190127@gmail.com</t>
+  </si>
+  <si>
     <t>Lê Thúy Ái</t>
   </si>
   <si>
+    <t>CS190640</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>AiLT.CS190640@gmail.com</t>
+  </si>
+  <si>
     <t>Nguyễn Thúy Thùy Linh</t>
   </si>
   <si>
+    <t>CE190669</t>
+  </si>
+  <si>
+    <t>LinhNTT.CE190669@gmail.com</t>
+  </si>
+  <si>
     <t>Lâm Quốc Minh</t>
   </si>
   <si>
+    <t>CE190585</t>
+  </si>
+  <si>
+    <t>MinhLQ.CE190585@gmail.com</t>
+  </si>
+  <si>
     <t>Nguyễn Thị Như Ngọc</t>
   </si>
   <si>
+    <t>CS190676</t>
+  </si>
+  <si>
+    <t>NgocNTN.CS190676@gmail.com</t>
+  </si>
+  <si>
     <t>Nguyễn Thị Kim Nhã</t>
   </si>
   <si>
+    <t>CE190530</t>
+  </si>
+  <si>
+    <t>NhaNTK.CE190530@gmail.com</t>
+  </si>
+  <si>
     <t>Lâm Triệu Phú</t>
   </si>
   <si>
+    <t>CE190365</t>
+  </si>
+  <si>
+    <t>PhuLT.CE190365@gmail.com</t>
+  </si>
+  <si>
     <t>Thiều Trần Quốc Quý</t>
   </si>
   <si>
+    <t>CE190497</t>
+  </si>
+  <si>
+    <t>QuyTTQ.CE190497@gmail.com</t>
+  </si>
+  <si>
     <t>Nguyễn Trúc Quỳnh</t>
   </si>
   <si>
+    <t>CE190172</t>
+  </si>
+  <si>
+    <t>QuynhNT.CE190172@gmail.com</t>
+  </si>
+  <si>
     <t>Nguyễn Thị Hoài Thương</t>
   </si>
   <si>
+    <t>CE190185</t>
+  </si>
+  <si>
+    <t>ThuongNTH.CE190185@gmail.com</t>
+  </si>
+  <si>
     <t>Nguyễn Thị Mộng Trúc</t>
   </si>
   <si>
+    <t>CA190426</t>
+  </si>
+  <si>
+    <t>TrucNTM.CA190426@gmail.com</t>
+  </si>
+  <si>
     <t>Hồ Phúc Vinh</t>
   </si>
   <si>
+    <t>CA190731</t>
+  </si>
+  <si>
+    <t>VinhHP.CA190731@gmail.com</t>
+  </si>
+  <si>
     <t>Nguyễn Hoàng Xuân Yến</t>
   </si>
   <si>
+    <t>CA190150</t>
+  </si>
+  <si>
+    <t>YenNHX.CA190150@gmail.com</t>
+  </si>
+  <si>
     <t>Trương Thành Công</t>
   </si>
   <si>
+    <t>CS190989</t>
+  </si>
+  <si>
+    <t>CongTT.CS190989@gmail.com</t>
+  </si>
+  <si>
     <t>Trần Trúc Mai Đào</t>
   </si>
   <si>
+    <t>CS190433</t>
+  </si>
+  <si>
+    <t>DaoTTM.CS190433@gmail.com</t>
+  </si>
+  <si>
     <t>Huỳnh Nhật Huy</t>
   </si>
   <si>
+    <t>CS191116</t>
+  </si>
+  <si>
+    <t>HuyHN.CS191116@gmail.com</t>
+  </si>
+  <si>
     <t>Võ Đăng Huy</t>
   </si>
   <si>
+    <t>CS190354</t>
+  </si>
+  <si>
+    <t>HuyVD.CS190354@gmail.com</t>
+  </si>
+  <si>
     <t>Trần Đăng Khoa</t>
   </si>
   <si>
+    <t>CE191209</t>
+  </si>
+  <si>
+    <t>KhoaTD.CE191209@gmail.com</t>
+  </si>
+  <si>
     <t>Huỳnh Tú Kiều</t>
   </si>
   <si>
+    <t>CS191269</t>
+  </si>
+  <si>
+    <t>KieuHT.CS191269@gmail.com</t>
+  </si>
+  <si>
     <t>Châu Triều Phát</t>
   </si>
   <si>
+    <t>CE191109</t>
+  </si>
+  <si>
+    <t>PhatCT.CE191109@gmail.com</t>
+  </si>
+  <si>
     <t>Nguyễn Phú Quý</t>
   </si>
   <si>
+    <t>CE191111</t>
+  </si>
+  <si>
+    <t>QuyNP.CE191111@gmail.com</t>
+  </si>
+  <si>
     <t>Tạ Ngọc Trân</t>
   </si>
   <si>
+    <t>CS191278</t>
+  </si>
+  <si>
+    <t>TranTN.CS191278@gmail.com</t>
+  </si>
+  <si>
     <t>Lê Ngô Hồng Ân</t>
   </si>
   <si>
+    <t>CS191563</t>
+  </si>
+  <si>
+    <t>AnLNH.CS191563@gmail.com</t>
+  </si>
+  <si>
     <t>Huỳnh Ngọc Trúc My</t>
   </si>
   <si>
+    <t>CA191546</t>
+  </si>
+  <si>
+    <t>MyHNT.CA191546@gmail.com</t>
+  </si>
+  <si>
     <t>Lý Phong Nhã</t>
   </si>
   <si>
+    <t>CE191118</t>
+  </si>
+  <si>
+    <t>NhaLP.CE191118@gmail.com</t>
+  </si>
+  <si>
     <t>Đỗ Thị Lâm Oanh</t>
   </si>
   <si>
+    <t>CS191643</t>
+  </si>
+  <si>
+    <t>OanhDTL.CS191643@gmail.com</t>
+  </si>
+  <si>
     <t>Dương Thị Kim Ngân</t>
   </si>
   <si>
+    <t>CS191700</t>
+  </si>
+  <si>
+    <t>NganDTK.CS191700@gmail.com</t>
+  </si>
+  <si>
     <t>Lê Huỳnh Thanh Phong</t>
   </si>
   <si>
-    <t>CE190127</t>
-  </si>
-  <si>
-    <t>CS190640</t>
-  </si>
-  <si>
-    <t>CE190669</t>
-  </si>
-  <si>
-    <t>CE190585</t>
-  </si>
-  <si>
-    <t>CS190676</t>
-  </si>
-  <si>
-    <t>CE190530</t>
-  </si>
-  <si>
-    <t>CE190365</t>
-  </si>
-  <si>
-    <t>CE190497</t>
-  </si>
-  <si>
-    <t>CE190172</t>
-  </si>
-  <si>
-    <t>CE190185</t>
-  </si>
-  <si>
-    <t>CA190426</t>
-  </si>
-  <si>
-    <t>CA190731</t>
-  </si>
-  <si>
-    <t>CA190150</t>
-  </si>
-  <si>
-    <t>CS190989</t>
-  </si>
-  <si>
-    <t>CS190433</t>
-  </si>
-  <si>
-    <t>CS191116</t>
-  </si>
-  <si>
-    <t>CS190354</t>
-  </si>
-  <si>
-    <t>CE191209</t>
-  </si>
-  <si>
-    <t>CS191269</t>
-  </si>
-  <si>
-    <t>CE191109</t>
-  </si>
-  <si>
-    <t>CE191111</t>
-  </si>
-  <si>
-    <t>CS191278</t>
-  </si>
-  <si>
-    <t>CS191563</t>
-  </si>
-  <si>
-    <t>CA191546</t>
-  </si>
-  <si>
-    <t>CE191118</t>
-  </si>
-  <si>
-    <t>CS191643</t>
-  </si>
-  <si>
-    <t>CS191700</t>
-  </si>
-  <si>
     <t>CS191306</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>AnhPD.CE190127@gmail.com</t>
-  </si>
-  <si>
-    <t>AiLT.CS190640@gmail.com</t>
-  </si>
-  <si>
-    <t>LinhNTT.CE190669@gmail.com</t>
-  </si>
-  <si>
-    <t>MinhLQ.CE190585@gmail.com</t>
-  </si>
-  <si>
-    <t>NgocNTN.CS190676@gmail.com</t>
-  </si>
-  <si>
-    <t>NhaNTK.CE190530@gmail.com</t>
-  </si>
-  <si>
-    <t>PhuLT.CE190365@gmail.com</t>
-  </si>
-  <si>
-    <t>QuyTTQ.CE190497@gmail.com</t>
-  </si>
-  <si>
-    <t>QuynhNT.CE190172@gmail.com</t>
-  </si>
-  <si>
-    <t>ThuongNTH.CE190185@gmail.com</t>
-  </si>
-  <si>
-    <t>TrucNTM.CA190426@gmail.com</t>
-  </si>
-  <si>
-    <t>VinhHP.CA190731@gmail.com</t>
-  </si>
-  <si>
-    <t>YenNHX.CA190150@gmail.com</t>
-  </si>
-  <si>
-    <t>CongTT.CS190989@gmail.com</t>
-  </si>
-  <si>
-    <t>DaoTTM.CS190433@gmail.com</t>
-  </si>
-  <si>
-    <t>HuyHN.CS191116@gmail.com</t>
-  </si>
-  <si>
-    <t>HuyVD.CS190354@gmail.com</t>
-  </si>
-  <si>
-    <t>KhoaTD.CE191209@gmail.com</t>
-  </si>
-  <si>
-    <t>KieuHT.CS191269@gmail.com</t>
-  </si>
-  <si>
-    <t>PhatCT.CE191109@gmail.com</t>
-  </si>
-  <si>
-    <t>QuyNP.CE191111@gmail.com</t>
-  </si>
-  <si>
-    <t>TranTN.CS191278@gmail.com</t>
-  </si>
-  <si>
-    <t>AnLNH.CS191563@gmail.com</t>
-  </si>
-  <si>
-    <t>MyHNT.CA191546@gmail.com</t>
-  </si>
-  <si>
-    <t>NhaLP.CE191118@gmail.com</t>
-  </si>
-  <si>
-    <t>OanhDTL.CS191643@gmail.com</t>
-  </si>
-  <si>
-    <t>NganDTK.CS191700@gmail.com</t>
-  </si>
-  <si>
     <t>PhongLHT.CS191306@gmail.com</t>
+  </si>
+  <si>
+    <t>Bach Ngoc Nhu</t>
+  </si>
+  <si>
+    <t>ca172063</t>
+  </si>
+  <si>
+    <t>nhubnca172063@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>Mã Cơ Sở</t>
+  </si>
+  <si>
+    <t>Tên Cơ sở</t>
   </si>
 </sst>
 </file>
@@ -893,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2873B9-7416-42AE-B6F0-05C25F416B1B}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -912,16 +928,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
@@ -932,102 +948,102 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21.75">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21.75">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21.75">
@@ -1035,39 +1051,39 @@
         <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21.75">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21.75">
@@ -1075,19 +1091,19 @@
         <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21.75">
@@ -1095,19 +1111,19 @@
         <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21.75">
@@ -1115,19 +1131,19 @@
         <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="21.75">
@@ -1135,19 +1151,19 @@
         <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="21.75">
@@ -1155,19 +1171,19 @@
         <v>48</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21.75">
@@ -1175,13 +1191,13 @@
         <v>51</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>54</v>
@@ -1195,13 +1211,13 @@
         <v>56</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>54</v>
@@ -1215,559 +1231,573 @@
         <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
         <v>99</v>
       </c>
-      <c r="C28" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" t="s">
-        <v>129</v>
-      </c>
       <c r="E28" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="B42" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>144</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1818,4 +1848,25 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId43"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036E444A-FD5B-4B73-965F-1E1C48D0623E}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified query in sql
</commit_message>
<xml_diff>
--- a/StudentList.xlsx
+++ b/StudentList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT University\DPI202\github\StudentManagementDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fptuniversity-my.sharepoint.com/personal/anhlnce181767_fpt_edu_vn/Documents/FPT University/2024/SP24/SE1804/DBI202/Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{7076F42A-1260-4E82-ADEA-54BA819E25A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6289FA8C-0C0E-4E90-89C0-0612DEA37F9D}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="8_{7076F42A-1260-4E82-ADEA-54BA819E25A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{301C1297-33C4-42D8-96CA-329D44DCFE69}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C5753F7D-290E-43CF-B893-8C0D3F93B633}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="227">
   <si>
     <t>họ và tên</t>
   </si>
@@ -222,9 +222,6 @@
     <t>CE190127</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>AnhPD.CE190127@gmail.com</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>CS190640</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>AiLT.CS190640@gmail.com</t>
   </si>
   <si>
@@ -487,13 +481,265 @@
   </si>
   <si>
     <t>Tên Cơ sở</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Hotline</t>
+  </si>
+  <si>
+    <t>FUHN</t>
+  </si>
+  <si>
+    <t>An Duc Nhat</t>
+  </si>
+  <si>
+    <t>FUQN</t>
+  </si>
+  <si>
+    <t>FUDN</t>
+  </si>
+  <si>
+    <t>FUHCM</t>
+  </si>
+  <si>
+    <t>nhatadhe180033@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>FUCT</t>
+  </si>
+  <si>
+    <t>Cần Thơ</t>
+  </si>
+  <si>
+    <t>TP.Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Đà Nẵng</t>
+  </si>
+  <si>
+    <t>Quy Nhơn</t>
+  </si>
+  <si>
+    <t>Hòa Lạc</t>
+  </si>
+  <si>
+    <t>Hoa Lac Hi-Tech Park, Km29 Thang Long Avenue, Thach That District, Hanoi</t>
+  </si>
+  <si>
+    <t>024 7300 6800</t>
+  </si>
+  <si>
+    <t>An Phu Thinh new urban area (in Dong Da ward and Nhon Binh ward)</t>
+  </si>
+  <si>
+    <t>he180033</t>
+  </si>
+  <si>
+    <t>(0256) 7300 999</t>
+  </si>
+  <si>
+    <t>FPT Da Nang urban area, Hoa Hai Ward, Ngu Hanh Son District, Da Nang City</t>
+  </si>
+  <si>
+    <t>(0236) 730 0999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No. 5 Nguyen Gia Thieu, District 3, Ho Chi Minh City (FSB Institute of Management and Technology facility)</t>
+  </si>
+  <si>
+    <t>(028) 7300 5588</t>
+  </si>
+  <si>
+    <t>Rau Ram Bridge, Area 6, extended Nguyen Van Cu, An Binh ward, Ninh Kieu district, city. Can Tho</t>
+  </si>
+  <si>
+    <t>(0292) 7773636</t>
+  </si>
+  <si>
+    <t>An Ha Yen Linh </t>
+  </si>
+  <si>
+    <t>linhahyhe186807@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>he186807</t>
+  </si>
+  <si>
+    <t>Bach Chau Loan</t>
+  </si>
+  <si>
+    <t>loanbche182593@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>Cở sở đào tạo</t>
+  </si>
+  <si>
+    <t>he182593</t>
+  </si>
+  <si>
+    <t>Chương trình đạo tào</t>
+  </si>
+  <si>
+    <t>Bach Hai Yen</t>
+  </si>
+  <si>
+    <t>yenbhhs180462@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>Mã chương trình</t>
+  </si>
+  <si>
+    <t>hs180462</t>
+  </si>
+  <si>
+    <t>Tên chương trình</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>Bach Van Duc</t>
+  </si>
+  <si>
+    <t>BIT</t>
+  </si>
+  <si>
+    <t>ducbvhe181874@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>Bachelor Program of Information Technology</t>
+  </si>
+  <si>
+    <t>he181874</t>
+  </si>
+  <si>
+    <t>General objective: Training Bachelor of Information Technology, Digital Art &amp; Design specialty with personality and capacity to meet the needs of society, mastering professional knowledge and practice, being able to organize, implement and promote the creativity in jobs related to the trained specialty, being able to work in the international environment, and laying the foundation to pursue further study and research in Digital Art &amp; Design.</t>
+  </si>
+  <si>
+    <t>Bui Anh Linh</t>
+  </si>
+  <si>
+    <t>linhbahe187296@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>BEN</t>
+  </si>
+  <si>
+    <t>Bachelor of English Studies</t>
+  </si>
+  <si>
+    <t>The bachelor's program in English Language aims to train good quality bachelors: with qualities and abilities to meet the actual needs of society; Able to use English fluently with a minimum level equivalent to level 5 according to The Vietnam Six-level of Foreign Language Proficiency Framework or level C1 according to the Common European Framework of Reference for Languages (CEFR) and Chinese with the minimum level is equivalent to HSK4 according to the six-level Chinese Proficiency Test or B2 level according to the Common European Framework of Reference for Languages (CEFR). Students have a strong self-study ability, are capable of self-training and accumulating professional knowledge, qualities, and skills to participate in the study, research at higher levels, or become experts in the field of expertise, flexible working in a domestic and international environment. Depending on the chosen major, students will be able to use Chinese as a second foreign language at a basic or intermediate level; have basic or advanced professional knowledge of languages and cultures; as well as the knowledge and skills necessary to work in fields related to the trained major.</t>
+  </si>
+  <si>
+    <t>BBA</t>
+  </si>
+  <si>
+    <t>Bachelor Program of Business Adminstration</t>
+  </si>
+  <si>
+    <t>he187296</t>
+  </si>
+  <si>
+    <t>The objective of the Bachelor of Business Administration – Tourism and Travel Management program of FPT University is to train students into specialists in tourism and travel management, tour guides, tour managers and operators. Students will be equipped with all essential knowledge and skills to work in the field of tourism and travel management and in an international working environment or to continue into the next higher level of education.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BJP </t>
+  </si>
+  <si>
+    <t>Bachelor Program of Japanese Studies</t>
+  </si>
+  <si>
+    <t>The professional objective of the Training program of Japanese Language (hereinafter referred to as the Training program) is to train Japanese Language graduates with political qualities, professional ethics, having an understanding of Japanese culture, mastering knowledge of Japanese language and being able to use Japanese as an effective tool at work. With 3 orientations namely Translation - Interpreting, Hotel &amp; Tourism Management, and Information Technology, students can develop careers in specialized fields and keep up with the development trends towards diversification and specialization of many fields and occupations of the society, meet demand for human resources related to Japanese language of agencies and departments organizations and enterprises in the domestic and foreign environment.
+In addition, the Training program always emphasizes on equipping students with foreign language skills through the Preparation English program lasting from 0-1 years depending on the student's level and the output is equivalent to IELTS 6.0. After graduating, students can study and work in international and multicultural environments in different countries.
+The training program also aims to provide students with soft skills such as communication, teamwork, critical thinking, entrepreneurial mindset, serious work spirit, dedication, creative thinking, the ability of lifelong learning and fundamental understandings of politics, law, ethics, and scientific methodology. These knowledge and skills will be equipped for students through the courses of Political theory, National Defense Education, etc.
+The program also aims to preserve the values and national identity of Vietnam by involving Traditional musical instruments, Vovinam courses in the training program. These values will help deepen students' national pride, bringing difference for learners when working in multicultural environments.</t>
+  </si>
+  <si>
+    <t>BKR</t>
+  </si>
+  <si>
+    <t>Bachelor Program of Korean studies</t>
+  </si>
+  <si>
+    <t>Training Bachelor of Korean Language with political qualities, professional ethics, having an understanding of Korean culture, master knowledge and language skills to apply fluently in a multilingual and multicultural environment. With 2 combos namely "Economy and Trade Orientation" and "Tourism Orientation", students will be equipped with supplemental knowledge and skills, having solid professional skills, meeting the needs of society and the Vietnamese economy which is developing and under the integration process into the global economy.</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>Preparation English</t>
+  </si>
+  <si>
+    <t>The preparation phase involves a 5-week Orientation and General Training program (OTP) and the English Preparation courses (PEN) which could last from 2 months to 1 year. The OTP includes 3 parts: 1) Orientation; 2) Military training; and 3) Experience, aiming at introducing students to community engagement, sustainable development, and military training. Students may have to attend PEN only if they fail to meet the entrance language requirement. PEN is classified into 6 levels ranging from A0 to B2 and each level of PEN is taught in 2 months. PEN could take place before or simultaneously with the OTP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEL </t>
+  </si>
+  <si>
+    <t>English Language</t>
+  </si>
+  <si>
+    <t>Training bachelors in English Language to have enough knowledge, professional skills, political products, ethics, professional behavior and good health to be able to work effectively through the use of English in the field. field of commerce or information technology, meeting the requirements of society and the economy in the process of international integration. Training program objectives: a) Equip students with basic knowledge of the English language, knowledge and professional skills in specific fields such as commerce or information technology. b) Train students in the necessary virtues and skills in a professional working environment, know how to apply language knowledge and combine knowledge of commerce and information technology into real work. c) Provide students with cultural and social knowledge; Train and promote initiative and creativity in study, work and life. Students majoring in English can work at domestic enterprises, foreign-invested enterprises, representative offices, international organizations, economic, financial, and public organizations. Domestic, international and regional arts in fields such as education, business, import-export, media, aviation, banking, auditing, management and research, can guarantee some jobs such as: - Translator, interpreter; - Sales, sales, business development officer; - Signal officer; - Transaction officer; - Teller - Customer care officer - Assistant (internship) director, project director; - English lecturer specializing in commerce and technology</t>
+  </si>
+  <si>
+    <t>BGD</t>
+  </si>
+  <si>
+    <t>Graphic Design</t>
+  </si>
+  <si>
+    <t>Buffet 1 &amp; 2 free
+ADI201 Design effective design (Brand identity design)
+ADB201 Design Book (Book Design)
+ADP201 Packaging design (Packaging design)
+DGP201 Digital Painting (Digital Painting)</t>
+  </si>
+  <si>
+    <t>BMC</t>
+  </si>
+  <si>
+    <t>Multimedia Communicatio</t>
+  </si>
+  <si>
+    <t>Elective industry knowledge group 1 (choose 2/4)
+WED201 Basic website design Web Design
+DTG302 Image and sound design in filmmaking (Visual Effects - Principles of Compositing)
+TPG20x Typography 1 (Typography 1)
+MID201 Multimedia Interactive Design (Multimedia Interactive Design)
+Elective industry knowledge group 2 (choose 2/3)
+MKT304 Integrated Marketing Communication
+CMC201 Culture and Communication (Communication and Culture)
+CAA201 Principles of Advertising and Communication (Principles of Advertising and Communication)</t>
+  </si>
+  <si>
+    <t>Bui Bao Linh</t>
+  </si>
+  <si>
+    <t>linhbbhe182407@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>he182407</t>
+  </si>
+  <si>
+    <t>Bui Bich Phuong</t>
+  </si>
+  <si>
+    <t>phuongbbhs186068@fpt.edu.vn</t>
+  </si>
+  <si>
+    <t>hs186068</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,9 +780,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF0B57D0"/>
-      <name val="Google Sans Text"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -560,7 +828,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -573,7 +841,32 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -590,6 +883,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -909,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2873B9-7416-42AE-B6F0-05C25F416B1B}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -920,7 +1217,7 @@
     <col min="1" max="1" width="39.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="3"/>
@@ -956,7 +1253,7 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -976,7 +1273,7 @@
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -996,7 +1293,7 @@
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1006,7 +1303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="21.75">
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -1016,47 +1313,47 @@
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="21.75">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="21.75">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="15" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1066,8 +1363,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="21.75">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1076,7 +1373,7 @@
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="15" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1086,8 +1383,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="21.75">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1096,18 +1393,18 @@
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="21.75">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1116,7 +1413,7 @@
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1126,8 +1423,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="21.75">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1136,7 +1433,7 @@
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1146,8 +1443,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="21.75">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1156,7 +1453,7 @@
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="15" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1166,8 +1463,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="21.75">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1176,7 +1473,7 @@
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="15" t="s">
         <v>50</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1186,8 +1483,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="21.75">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1196,7 +1493,7 @@
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="15" t="s">
         <v>53</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1206,8 +1503,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="21.75">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1216,7 +1513,7 @@
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="15" t="s">
         <v>58</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1227,17 +1524,17 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>61</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>10</v>
@@ -1247,17 +1544,17 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>10</v>
@@ -1267,17 +1564,17 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>10</v>
@@ -1287,17 +1584,17 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
@@ -1307,17 +1604,17 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" t="s">
-        <v>75</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>10</v>
@@ -1327,17 +1624,17 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>10</v>
@@ -1347,17 +1644,17 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" t="s">
-        <v>81</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>10</v>
@@ -1367,17 +1664,17 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" t="s">
-        <v>84</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>10</v>
@@ -1387,17 +1684,17 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" t="s">
-        <v>87</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>10</v>
@@ -1407,17 +1704,17 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" t="s">
-        <v>90</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>10</v>
@@ -1427,17 +1724,17 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" t="s">
-        <v>93</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>10</v>
@@ -1447,17 +1744,17 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" t="s">
-        <v>96</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>10</v>
@@ -1467,17 +1764,17 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" t="s">
-        <v>99</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>10</v>
@@ -1487,17 +1784,17 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" t="s">
-        <v>102</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>10</v>
@@ -1507,17 +1804,17 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B30" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" t="s">
-        <v>105</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>10</v>
@@ -1527,17 +1824,17 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" t="s">
-        <v>108</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>10</v>
@@ -1547,17 +1844,17 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>109</v>
-      </c>
-      <c r="B32" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>10</v>
@@ -1567,17 +1864,17 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="B33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>10</v>
@@ -1587,17 +1884,17 @@
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="B34" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>10</v>
@@ -1607,17 +1904,17 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" t="s">
+      <c r="A35" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>118</v>
-      </c>
-      <c r="B35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>10</v>
@@ -1627,17 +1924,17 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="B36" t="s">
-        <v>122</v>
-      </c>
-      <c r="C36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>10</v>
@@ -1647,17 +1944,17 @@
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="B37" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>126</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>10</v>
@@ -1667,17 +1964,17 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" t="s">
+      <c r="A38" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="B38" t="s">
-        <v>128</v>
-      </c>
-      <c r="C38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>10</v>
@@ -1687,17 +1984,17 @@
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" t="s">
+      <c r="A39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>130</v>
-      </c>
-      <c r="B39" t="s">
-        <v>131</v>
-      </c>
-      <c r="C39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>10</v>
@@ -1707,17 +2004,17 @@
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" t="s">
+      <c r="A40" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="B40" t="s">
-        <v>134</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>135</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>10</v>
@@ -1727,17 +2024,17 @@
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" t="s">
+      <c r="A41" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>136</v>
-      </c>
-      <c r="B41" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>10</v>
@@ -1747,17 +2044,17 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>139</v>
-      </c>
-      <c r="B42" t="s">
-        <v>140</v>
-      </c>
-      <c r="C42" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>10</v>
@@ -1767,17 +2064,17 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="15" t="s">
         <v>142</v>
-      </c>
-      <c r="B43" t="s">
-        <v>143</v>
-      </c>
-      <c r="C43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>10</v>
@@ -1788,16 +2085,182 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>147</v>
+      <c r="E44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="21.75">
+      <c r="A51" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="21.75">
+      <c r="A52" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1844,29 +2307,252 @@
     <hyperlink ref="D40" r:id="rId40" xr:uid="{5C71402B-CF76-4386-914F-26D1A945DFE6}"/>
     <hyperlink ref="D42" r:id="rId41" xr:uid="{EB8C1750-A792-47B0-9FD7-EB831BCECCD7}"/>
     <hyperlink ref="D43" r:id="rId42" xr:uid="{6DDF8426-484F-465E-AA3B-C9C6C63C18E6}"/>
+    <hyperlink ref="D45" r:id="rId43" xr:uid="{050A9ADE-88A5-4C51-B33A-24F036E5E8CF}"/>
+    <hyperlink ref="D44" r:id="rId44" xr:uid="{9EFFD5FF-2F01-4100-94F4-58179B7135B8}"/>
+    <hyperlink ref="D46" r:id="rId45" xr:uid="{2EBE345D-67E5-4B19-8BCD-D302C2705FC5}"/>
+    <hyperlink ref="D47" r:id="rId46" xr:uid="{34DBF009-EA45-46DD-8632-0D00D56A724A}"/>
+    <hyperlink ref="D48" r:id="rId47" xr:uid="{36A982E2-EE75-4E49-8568-397769CB103F}"/>
+    <hyperlink ref="D49" r:id="rId48" xr:uid="{91FB4077-EE5A-4527-9EE2-3F46F6022AE5}"/>
+    <hyperlink ref="D51" r:id="rId49" xr:uid="{8F79D9C2-CD7C-4879-B603-01D71F6BE3CC}"/>
+    <hyperlink ref="D52" r:id="rId50" xr:uid="{FF07D874-6C80-49DB-ACD3-3CC442EF9210}"/>
+    <hyperlink ref="D50" r:id="rId51" xr:uid="{BC890A6D-E0C2-458B-BEE0-2BEEA63C311C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId43"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId52"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036E444A-FD5B-4B73-965F-1E1C48D0623E}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" s="9" t="s">
         <v>149</v>
       </c>
     </row>
+    <row r="3" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45">
+      <c r="A7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="150">
+      <c r="A11" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="390">
+      <c r="A12" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="150">
+      <c r="A13" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="409.5">
+      <c r="A14" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="195">
+      <c r="A15" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="210">
+      <c r="A16" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="409.5">
+      <c r="A17" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="105">
+      <c r="A18" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="210">
+      <c r="A19" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A9:D9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update query in student management database
</commit_message>
<xml_diff>
--- a/StudentList.xlsx
+++ b/StudentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fptuniversity-my.sharepoint.com/personal/anhlnce181767_fpt_edu_vn/Documents/FPT University/2024/SP24/SE1804/DBI202/Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="8_{7076F42A-1260-4E82-ADEA-54BA819E25A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{301C1297-33C4-42D8-96CA-329D44DCFE69}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{7076F42A-1260-4E82-ADEA-54BA819E25A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2654B15A-CE23-4BC3-974C-686D18CBEBD7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C5753F7D-290E-43CF-B893-8C0D3F93B633}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C5753F7D-290E-43CF-B893-8C0D3F93B633}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,9 +639,6 @@
     <t>BBA</t>
   </si>
   <si>
-    <t>Bachelor Program of Business Adminstration</t>
-  </si>
-  <si>
     <t>he187296</t>
   </si>
   <si>
@@ -733,6 +730,9 @@
   </si>
   <si>
     <t>hs186068</t>
+  </si>
+  <si>
+    <t>Bachelor Program of Business Administration</t>
   </si>
 </sst>
 </file>
@@ -847,16 +847,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -866,6 +860,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -883,10 +883,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1208,22 +1204,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2873B9-7416-42AE-B6F0-05C25F416B1B}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="39.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1249,7 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1273,7 +1269,7 @@
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1293,7 +1289,7 @@
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1313,7 +1309,7 @@
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="13" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -1327,13 +1323,13 @@
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1353,7 +1349,7 @@
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="13" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1373,7 +1369,7 @@
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="13" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1393,7 +1389,7 @@
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="13" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1413,7 +1409,7 @@
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="13" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1433,7 +1429,7 @@
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="13" t="s">
         <v>44</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1453,7 +1449,7 @@
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="13" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1473,7 +1469,7 @@
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="13" t="s">
         <v>50</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1493,7 +1489,7 @@
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="13" t="s">
         <v>53</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1513,7 +1509,7 @@
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="13" t="s">
         <v>58</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1533,7 +1529,7 @@
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="13" t="s">
         <v>61</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1553,7 +1549,7 @@
       <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="13" t="s">
         <v>64</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1573,7 +1569,7 @@
       <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="13" t="s">
         <v>67</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1853,7 +1849,7 @@
       <c r="C32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="13" t="s">
         <v>109</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1873,7 +1869,7 @@
       <c r="C33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="13" t="s">
         <v>112</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1893,7 +1889,7 @@
       <c r="C34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="13" t="s">
         <v>115</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -1913,7 +1909,7 @@
       <c r="C35" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="13" t="s">
         <v>118</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1933,7 +1929,7 @@
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="13" t="s">
         <v>121</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1953,7 +1949,7 @@
       <c r="C37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="13" t="s">
         <v>124</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -1973,7 +1969,7 @@
       <c r="C38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="13" t="s">
         <v>127</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1993,7 +1989,7 @@
       <c r="C39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="13" t="s">
         <v>130</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -2013,7 +2009,7 @@
       <c r="C40" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="13" t="s">
         <v>133</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -2033,7 +2029,7 @@
       <c r="C41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="13" t="s">
         <v>136</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -2053,7 +2049,7 @@
       <c r="C42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="13" t="s">
         <v>139</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -2073,7 +2069,7 @@
       <c r="C43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="13" t="s">
         <v>142</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -2093,7 +2089,7 @@
       <c r="C44" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="13" t="s">
         <v>145</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -2113,7 +2109,7 @@
       <c r="C45" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="13" t="s">
         <v>155</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -2133,7 +2129,7 @@
       <c r="C46" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="13" t="s">
         <v>174</v>
       </c>
       <c r="E46" s="5" t="s">
@@ -2153,7 +2149,7 @@
       <c r="C47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="13" t="s">
         <v>177</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -2173,7 +2169,7 @@
       <c r="C48" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="13" t="s">
         <v>182</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2193,7 +2189,7 @@
       <c r="C49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="13" t="s">
         <v>190</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -2207,8 +2203,8 @@
       <c r="A50" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B50" s="16" t="s">
-        <v>201</v>
+      <c r="B50" s="14" t="s">
+        <v>200</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>8</v>
@@ -2223,18 +2219,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="21.75">
+    <row r="51" spans="1:6" ht="21">
       <c r="A51" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>54</v>
@@ -2243,18 +2239,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="21.75">
+    <row r="52" spans="1:6" ht="21">
       <c r="A52" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>224</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>225</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>54</v>
@@ -2326,25 +2322,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036E444A-FD5B-4B73-965F-1E1C48D0623E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
@@ -2388,7 +2384,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="28.8">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -2402,7 +2398,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="28.8">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -2416,7 +2412,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45">
+    <row r="7" spans="1:4" ht="28.8">
       <c r="A7" t="s">
         <v>156</v>
       </c>
@@ -2431,12 +2427,12 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="9" t="s">
@@ -2449,103 +2445,103 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="150">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:4" ht="129.6">
+      <c r="A11" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>191</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="390">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:4" ht="345.6">
+      <c r="A12" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="150">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:4" ht="129.6">
+      <c r="A13" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>200</v>
+      <c r="B13" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="409.6">
+      <c r="A14" s="10" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="409.5">
-      <c r="A14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C14" s="8" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="158.4">
+      <c r="A15" s="10" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="195">
-      <c r="A15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="C15" s="17" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="172.8">
+      <c r="A16" s="11" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="210">
-      <c r="A16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="C16" s="17" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="409.6">
+      <c r="A17" s="11" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="409.5">
-      <c r="A17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="C17" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="C17" s="17" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="86.4">
+      <c r="A18" s="11" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="105">
-      <c r="A18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="C18" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="C18" s="17" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="187.2">
+      <c r="A19" s="11" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="210">
-      <c r="A19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="C19" s="15" t="s">
         <v>219</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>